<commit_message>
Post: DB update, corrected code accordingly
</commit_message>
<xml_diff>
--- a/data/post2002DB-v2.xlsx
+++ b/data/post2002DB-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hildad/Documents/GitHub/lyingpendatabases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB28C8-9217-B848-B4CD-1CF4D8EED686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC6DFC4-0A56-1F42-ACAA-8DEA50007AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{CB7DAB00-11D3-3A4F-BDDA-5DEC01C2CC59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{CB7DAB00-11D3-3A4F-BDDA-5DEC01C2CC59}"/>
   </bookViews>
   <sheets>
     <sheet name="Database of Post-2002 Fragments" sheetId="1" r:id="rId1"/>
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="626">
   <si>
     <t>No.</t>
   </si>
@@ -5602,9 +5602,6 @@
     <t>Instr1</t>
   </si>
   <si>
-    <t>4Q418 ii 4–5</t>
-  </si>
-  <si>
     <t xml:space="preserve">MOTB.SCR.000123
 </t>
   </si>
@@ -5770,9 +5767,6 @@
       </rPr>
       <t>. Volume 2. Jerusalem, 174.</t>
     </r>
-  </si>
-  <si>
-    <t>“4Q418”</t>
   </si>
   <si>
     <t>W 16</t>
@@ -6454,9 +6448,6 @@
     <t>Content group</t>
   </si>
   <si>
-    <t>Others</t>
-  </si>
-  <si>
     <t>Genesis, 1</t>
   </si>
   <si>
@@ -6518,12 +6509,6 @@
   </si>
   <si>
     <t>Micah, 21</t>
-  </si>
-  <si>
-    <t>Others, 22</t>
-  </si>
-  <si>
-    <t>Unidentified, 23</t>
   </si>
   <si>
     <t>Cluster of miniscule pieces</t>
@@ -6837,6 +6822,39 @@
   </si>
   <si>
     <t>Writings</t>
+  </si>
+  <si>
+    <t>Instruction (4Q418 ii 4–5)</t>
+  </si>
+  <si>
+    <t>Instruction (“4Q418”)</t>
+  </si>
+  <si>
+    <t>Tobit, 22</t>
+  </si>
+  <si>
+    <t>Apocrypha</t>
+  </si>
+  <si>
+    <t>1Enoch, 23</t>
+  </si>
+  <si>
+    <t>Pseudepigrapha</t>
+  </si>
+  <si>
+    <t>Instruction, 24</t>
+  </si>
+  <si>
+    <t>Qumran texts</t>
+  </si>
+  <si>
+    <t>Temple Scroll, 25</t>
+  </si>
+  <si>
+    <t>Commentary on Genesis, 26</t>
+  </si>
+  <si>
+    <t>Unidentified, 27</t>
   </si>
 </sst>
 </file>
@@ -7843,7 +7861,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4CEA2365-8B2D-5143-803D-6D4FB4E86B2D}" name="Post_2002_Fragments" displayName="Post_2002_Fragments" ref="A1:V102" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="A1:V102" xr:uid="{714D2FCE-A08D-C943-80D3-6D216A6BD6AA}"/>
+  <autoFilter ref="A1:V102" xr:uid="{714D2FCE-A08D-C943-80D3-6D216A6BD6AA}">
+    <filterColumn colId="20">
+      <filters>
+        <filter val="Unidentified, 23"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T102">
     <sortCondition ref="A1:A102"/>
   </sortState>
@@ -8238,9 +8262,9 @@
   </sheetPr>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V98" sqref="V98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8307,16 +8331,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>8</v>
@@ -8328,7 +8352,7 @@
         <v>10</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>11</v>
@@ -8343,13 +8367,13 @@
         <v>14</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="168" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="168" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -8398,13 +8422,13 @@
         <v>25</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="150" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="150" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -8427,7 +8451,7 @@
         <v>29</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>30</v>
@@ -8439,10 +8463,10 @@
         <v>32</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="N3" s="15" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="O3" s="15" t="s">
         <v>33</v>
@@ -8463,13 +8487,13 @@
         <v>38</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="408" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -8491,7 +8515,7 @@
       </c>
       <c r="G4" s="7"/>
       <c r="H4" s="25" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="7"/>
@@ -8516,13 +8540,13 @@
         <v>45</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="83" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="83" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -8564,21 +8588,21 @@
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
       <c r="T5" s="24" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="117.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C6" s="14">
         <v>101</v>
@@ -8624,13 +8648,13 @@
         <v>62</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" ht="221.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -8655,7 +8679,7 @@
         <v>66</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="J7" s="23"/>
       <c r="K7" s="17"/>
@@ -8681,13 +8705,13 @@
         <v>72</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="105.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" ht="105.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -8732,13 +8756,13 @@
         <v>80</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V8" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -8771,13 +8795,13 @@
         <v>82</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" ht="99.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -8828,13 +8852,13 @@
         <v>92</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="156.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="156.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -8859,7 +8883,7 @@
         <v>96</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="J11" s="7" t="s">
         <v>88</v>
@@ -8885,13 +8909,13 @@
         <v>100</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -8924,13 +8948,13 @@
         <v>82</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -8967,13 +8991,13 @@
         <v>105</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -9006,13 +9030,13 @@
         <v>82</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9061,13 +9085,13 @@
         <v>114</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="16" spans="1:22" ht="54" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="54" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -9112,10 +9136,10 @@
         <v>121</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -9167,13 +9191,13 @@
         <v>131</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -9220,13 +9244,13 @@
         <v>139</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -9259,13 +9283,13 @@
       <c r="S19" s="15"/>
       <c r="T19" s="21"/>
       <c r="U19" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -9310,13 +9334,13 @@
         <v>148</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9349,13 +9373,13 @@
         <v>82</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V21" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="81" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:22" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -9408,13 +9432,13 @@
         <v>157</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:22" ht="75" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -9459,13 +9483,13 @@
         <v>164</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -9506,13 +9530,13 @@
       <c r="S24" s="15"/>
       <c r="T24" s="21"/>
       <c r="U24" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V24" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9563,13 +9587,13 @@
         <v>180</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="26" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9620,18 +9644,18 @@
         <v>180</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="27" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="C27" s="14"/>
       <c r="D27" s="15"/>
@@ -9669,13 +9693,13 @@
         <v>180</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>595</v>
+        <v>573</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>573</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9708,13 +9732,13 @@
         <v>82</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V28" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9747,13 +9771,13 @@
         <v>82</v>
       </c>
       <c r="U29" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V29" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9796,13 +9820,13 @@
         <v>195</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V30" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9835,13 +9859,13 @@
         <v>82</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V31" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="32" spans="1:22" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:22" ht="119.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -9868,7 +9892,7 @@
         <v>201</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="J32" s="7"/>
       <c r="K32" s="15"/>
@@ -9892,13 +9916,13 @@
         <v>203</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9931,13 +9955,13 @@
         <v>82</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -9988,13 +10012,13 @@
         <v>213</v>
       </c>
       <c r="U34" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V34" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="35" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -10039,13 +10063,13 @@
         <v>148</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="36" spans="1:22" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:22" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -10068,7 +10092,7 @@
         <v>135</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="J36" s="7" t="s">
         <v>222</v>
@@ -10092,13 +10116,13 @@
         <v>226</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="37" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:22" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -10145,13 +10169,13 @@
         <v>234</v>
       </c>
       <c r="U37" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10184,13 +10208,13 @@
         <v>82</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V38" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:22" ht="97.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -10210,7 +10234,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="15"/>
       <c r="I39" s="15" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="J39" s="7" t="s">
         <v>238</v>
@@ -10222,10 +10246,10 @@
         <v>32</v>
       </c>
       <c r="M39" s="15" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="N39" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="O39" s="15" t="s">
         <v>22</v>
@@ -10240,13 +10264,13 @@
         <v>241</v>
       </c>
       <c r="U39" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V39" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="40" spans="1:22" ht="388.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:22" ht="388.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -10282,7 +10306,7 @@
         <v>248</v>
       </c>
       <c r="N40" s="15" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="O40" s="15" t="s">
         <v>33</v>
@@ -10297,13 +10321,13 @@
         <v>250</v>
       </c>
       <c r="U40" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V40" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="41" spans="1:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:22" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -10336,13 +10360,13 @@
         <v>82</v>
       </c>
       <c r="U41" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V41" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="42" spans="1:22" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:22" ht="119.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -10391,13 +10415,13 @@
         <v>258</v>
       </c>
       <c r="U42" s="1" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="V42" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
-    <row r="43" spans="1:22" ht="50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:22" ht="50" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10442,13 +10466,13 @@
         <v>267</v>
       </c>
       <c r="U43" s="15" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="V43" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10493,13 +10517,13 @@
         <v>275</v>
       </c>
       <c r="U44" s="15" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="V44" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10532,13 +10556,13 @@
         <v>82</v>
       </c>
       <c r="U45" s="15" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="V45" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10575,13 +10599,13 @@
       <c r="S46" s="15"/>
       <c r="T46" s="21"/>
       <c r="U46" s="15" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="V46" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:22" ht="33" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -10628,13 +10652,13 @@
         <v>288</v>
       </c>
       <c r="U47" s="15" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="V47" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="48" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:22" ht="40" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -10679,13 +10703,13 @@
         <v>295</v>
       </c>
       <c r="U48" s="15" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="V48" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="49" spans="1:22" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:22" ht="119.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -10734,13 +10758,13 @@
         <v>300</v>
       </c>
       <c r="U49" s="15" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="V49" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="50" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10773,13 +10797,13 @@
         <v>82</v>
       </c>
       <c r="U50" s="15" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="V50" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="51" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10830,13 +10854,13 @@
         <v>309</v>
       </c>
       <c r="U51" s="15" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="V51" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="52" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10877,13 +10901,13 @@
         <v>314</v>
       </c>
       <c r="U52" s="15" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="V52" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="53" spans="1:22" ht="119.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:22" ht="119.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>52</v>
       </c>
@@ -10930,13 +10954,13 @@
         <v>321</v>
       </c>
       <c r="U53" s="15" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="V53" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="54" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -10969,13 +10993,13 @@
         <v>82</v>
       </c>
       <c r="U54" s="15" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="V54" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="55" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:22" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>54</v>
       </c>
@@ -11008,13 +11032,13 @@
         <v>82</v>
       </c>
       <c r="U55" s="15" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="V55" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="56" spans="1:22" ht="60" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:22" ht="60" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -11057,13 +11081,13 @@
         <v>328</v>
       </c>
       <c r="U56" s="15" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="V56" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="57" spans="1:22" ht="167.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:22" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>56</v>
       </c>
@@ -11085,7 +11109,7 @@
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="25" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="I57" s="15"/>
       <c r="J57" s="7" t="s">
@@ -11114,13 +11138,13 @@
         <v>336</v>
       </c>
       <c r="U57" s="15" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="V57" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="58" spans="1:22" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:22" ht="84.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>57</v>
       </c>
@@ -11169,13 +11193,13 @@
         <v>344</v>
       </c>
       <c r="U58" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V58" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="59" spans="1:22" ht="169.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:22" ht="169.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>58</v>
       </c>
@@ -11230,13 +11254,13 @@
         <v>356</v>
       </c>
       <c r="U59" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V59" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="60" spans="1:22" ht="99" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:22" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>59</v>
       </c>
@@ -11255,7 +11279,7 @@
         <v>358</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="J60" s="8" t="s">
         <v>359</v>
@@ -11279,13 +11303,13 @@
         <v>362</v>
       </c>
       <c r="U60" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V60" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="61" spans="1:22" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:22" ht="87" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>60</v>
       </c>
@@ -11315,7 +11339,7 @@
       <c r="J61" s="7"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="M61" s="15"/>
       <c r="N61" s="15" t="s">
@@ -11334,13 +11358,13 @@
         <v>369</v>
       </c>
       <c r="U61" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V61" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="62" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -11373,13 +11397,13 @@
         <v>82</v>
       </c>
       <c r="U62" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V62" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="63" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -11414,13 +11438,13 @@
         <v>373</v>
       </c>
       <c r="U63" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V63" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="64" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:22" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>63</v>
       </c>
@@ -11453,13 +11477,13 @@
         <v>82</v>
       </c>
       <c r="U64" s="15" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="V64" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="65" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -11504,13 +11528,13 @@
         <v>380</v>
       </c>
       <c r="U65" s="15" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="V65" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="66" spans="1:22" ht="136.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:22" ht="136.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>65</v>
       </c>
@@ -11531,7 +11555,7 @@
         <v>29</v>
       </c>
       <c r="I66" s="15" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="J66" s="7" t="s">
         <v>383</v>
@@ -11543,10 +11567,10 @@
         <v>32</v>
       </c>
       <c r="M66" s="15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="N66" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="O66" s="15" t="s">
         <v>112</v>
@@ -11563,13 +11587,13 @@
         <v>387</v>
       </c>
       <c r="U66" s="15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="V66" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="67" spans="1:22" ht="153" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:22" ht="153" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -11590,7 +11614,7 @@
         <v>390</v>
       </c>
       <c r="I67" s="15" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="J67" s="7" t="s">
         <v>383</v>
@@ -11602,10 +11626,10 @@
         <v>32</v>
       </c>
       <c r="M67" s="15" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="N67" s="15" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="O67" s="15" t="s">
         <v>98</v>
@@ -11619,16 +11643,16 @@
       <c r="R67" s="15"/>
       <c r="S67" s="15"/>
       <c r="T67" s="24" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="U67" s="15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="V67" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="68" spans="1:22" ht="90" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:22" ht="90" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>67</v>
       </c>
@@ -11667,13 +11691,13 @@
         <v>397</v>
       </c>
       <c r="U68" s="15" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="V68" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="69" spans="1:22" ht="165" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:22" ht="165" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -11726,13 +11750,13 @@
         <v>405</v>
       </c>
       <c r="U69" s="15" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="V69" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="70" spans="1:22" ht="80" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:22" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -11777,13 +11801,13 @@
         <v>412</v>
       </c>
       <c r="U70" s="15" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="V70" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="71" spans="1:22" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:22" ht="114" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>70</v>
       </c>
@@ -11806,7 +11830,7 @@
         <v>415</v>
       </c>
       <c r="I71" s="15" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="J71" s="7" t="s">
         <v>416</v>
@@ -11834,13 +11858,13 @@
         <v>420</v>
       </c>
       <c r="U71" s="15" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="V71" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="72" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -11883,13 +11907,13 @@
         <v>426</v>
       </c>
       <c r="U72" s="15" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="V72" s="1" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
     </row>
-    <row r="73" spans="1:22" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:22" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>72</v>
       </c>
@@ -11938,13 +11962,13 @@
         <v>434</v>
       </c>
       <c r="U73" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V73" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="74" spans="1:22" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:22" ht="81.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>73</v>
       </c>
@@ -11991,13 +12015,13 @@
         <v>440</v>
       </c>
       <c r="U74" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V74" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="75" spans="1:22" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:22" ht="85.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>74</v>
       </c>
@@ -12040,13 +12064,13 @@
         <v>444</v>
       </c>
       <c r="U75" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V75" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="76" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -12089,13 +12113,13 @@
         <v>449</v>
       </c>
       <c r="U76" s="15" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="V76" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="77" spans="1:22" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:22" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -12128,13 +12152,13 @@
         <v>82</v>
       </c>
       <c r="U77" s="15" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="V77" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="78" spans="1:22" ht="50" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:22" ht="50" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -12171,13 +12195,13 @@
         <v>453</v>
       </c>
       <c r="U78" s="15" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="V78" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="79" spans="1:22" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:22" ht="69.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>78</v>
       </c>
@@ -12214,13 +12238,13 @@
         <v>457</v>
       </c>
       <c r="U79" s="15" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="V79" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="80" spans="1:22" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:22" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>79</v>
       </c>
@@ -12265,13 +12289,13 @@
         <v>464</v>
       </c>
       <c r="U80" s="15" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="V80" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="81" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -12304,13 +12328,13 @@
         <v>82</v>
       </c>
       <c r="U81" s="15" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="V81" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="82" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -12353,13 +12377,13 @@
         <v>471</v>
       </c>
       <c r="U82" s="15" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="V82" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="83" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -12402,13 +12426,13 @@
         <v>476</v>
       </c>
       <c r="U83" s="15" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="V83" s="1" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
-    <row r="84" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>83</v>
       </c>
@@ -12443,13 +12467,13 @@
       <c r="S84" s="15"/>
       <c r="T84" s="21"/>
       <c r="U84" s="15" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="V84" s="1" t="s">
-        <v>573</v>
+        <v>618</v>
       </c>
     </row>
-    <row r="85" spans="1:22" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:22" ht="122.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <v>84</v>
       </c>
@@ -12472,7 +12496,7 @@
       <c r="G85" s="7"/>
       <c r="H85" s="15"/>
       <c r="I85" s="15" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="J85" s="9" t="s">
         <v>483</v>
@@ -12495,16 +12519,16 @@
       <c r="R85" s="15"/>
       <c r="S85" s="15"/>
       <c r="T85" s="24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="U85" s="15" t="s">
-        <v>595</v>
+        <v>617</v>
       </c>
       <c r="V85" s="1" t="s">
-        <v>573</v>
+        <v>618</v>
       </c>
     </row>
-    <row r="86" spans="1:22" ht="80" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:22" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -12527,7 +12551,7 @@
       <c r="G86" s="7"/>
       <c r="H86" s="15"/>
       <c r="I86" s="15" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="J86" s="7" t="s">
         <v>489</v>
@@ -12551,13 +12575,13 @@
         <v>491</v>
       </c>
       <c r="U86" s="15" t="s">
-        <v>595</v>
+        <v>619</v>
       </c>
       <c r="V86" s="1" t="s">
-        <v>573</v>
+        <v>620</v>
       </c>
     </row>
-    <row r="87" spans="1:22" ht="159" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:22" ht="159" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>86</v>
       </c>
@@ -12608,13 +12632,13 @@
         <v>500</v>
       </c>
       <c r="U87" s="15" t="s">
-        <v>595</v>
+        <v>619</v>
       </c>
       <c r="V87" s="1" t="s">
-        <v>573</v>
+        <v>620</v>
       </c>
     </row>
-    <row r="88" spans="1:22" ht="30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:22" ht="30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -12661,18 +12685,18 @@
         <v>508</v>
       </c>
       <c r="U88" s="15" t="s">
-        <v>595</v>
+        <v>619</v>
       </c>
       <c r="V88" s="1" t="s">
-        <v>573</v>
+        <v>620</v>
       </c>
     </row>
-    <row r="89" spans="1:22" ht="200" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:22" ht="200" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>88</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>510</v>
+        <v>615</v>
       </c>
       <c r="C89" s="14">
         <v>202</v>
@@ -12685,19 +12709,19 @@
         <v>DSS F.202 Instr1</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G89" s="7"/>
       <c r="H89" s="15"/>
       <c r="I89" s="15" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="J89" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K89" s="15"/>
       <c r="L89" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="M89" s="15"/>
       <c r="N89" s="15"/>
@@ -12705,42 +12729,42 @@
         <v>112</v>
       </c>
       <c r="P89" s="15" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q89" s="7" t="s">
         <v>240</v>
       </c>
       <c r="R89" s="15" t="s">
+        <v>514</v>
+      </c>
+      <c r="S89" s="15" t="s">
         <v>515</v>
       </c>
-      <c r="S89" s="15" t="s">
+      <c r="T89" s="21" t="s">
         <v>516</v>
       </c>
-      <c r="T89" s="21" t="s">
-        <v>517</v>
-      </c>
       <c r="U89" s="15" t="s">
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
-    <row r="90" spans="1:22" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:22" ht="55" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>89</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>518</v>
+        <v>616</v>
       </c>
       <c r="C90" s="14"/>
       <c r="D90" s="15"/>
       <c r="E90" s="10" t="str">
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
-        <v>“4Q418”</v>
+        <v>Instruction (“4Q418”)</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="G90" s="7"/>
       <c r="H90" s="15"/>
@@ -12748,7 +12772,7 @@
       <c r="J90" s="7"/>
       <c r="K90" s="15"/>
       <c r="L90" s="15" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="M90" s="15"/>
       <c r="N90" s="15"/>
@@ -12758,21 +12782,21 @@
       <c r="R90" s="15"/>
       <c r="S90" s="15"/>
       <c r="T90" s="21" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="U90" s="15" t="s">
-        <v>595</v>
+        <v>621</v>
       </c>
       <c r="V90" s="1" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
-    <row r="91" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>90</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C91" s="14"/>
       <c r="D91" s="15"/>
@@ -12784,12 +12808,12 @@
       <c r="G91" s="7"/>
       <c r="H91" s="15"/>
       <c r="I91" s="15" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="J91" s="7"/>
       <c r="K91" s="15"/>
       <c r="L91" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
@@ -12800,18 +12824,18 @@
       <c r="S91" s="15"/>
       <c r="T91" s="21"/>
       <c r="U91" s="15" t="s">
-        <v>595</v>
+        <v>623</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
-    <row r="92" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>91</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C92" s="14"/>
       <c r="D92" s="15"/>
@@ -12823,54 +12847,54 @@
       <c r="G92" s="7"/>
       <c r="H92" s="15"/>
       <c r="I92" s="15" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="J92" s="7"/>
       <c r="K92" s="15"/>
       <c r="L92" s="15" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="M92" s="15"/>
       <c r="N92" s="15"/>
       <c r="O92" s="15"/>
       <c r="P92" s="15" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="Q92" s="7"/>
       <c r="R92" s="15"/>
       <c r="S92" s="15"/>
       <c r="T92" s="21"/>
       <c r="U92" s="15" t="s">
-        <v>595</v>
+        <v>623</v>
       </c>
       <c r="V92" s="1" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
-    <row r="93" spans="1:22" ht="45" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:22" ht="45" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <v>92</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C93" s="14">
         <v>130</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E93" s="10" t="str">
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.130 CommGen</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="G93" s="7"/>
       <c r="H93" s="15"/>
       <c r="I93" s="15" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J93" s="7"/>
       <c r="K93" s="15"/>
@@ -12883,17 +12907,17 @@
         <v>112</v>
       </c>
       <c r="P93" s="15" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="Q93" s="7"/>
       <c r="R93" s="15"/>
       <c r="S93" s="15"/>
       <c r="T93" s="21"/>
       <c r="U93" s="15" t="s">
-        <v>595</v>
+        <v>624</v>
       </c>
       <c r="V93" s="1" t="s">
-        <v>573</v>
+        <v>622</v>
       </c>
     </row>
     <row r="94" spans="1:22" ht="30" x14ac:dyDescent="0.2">
@@ -12901,7 +12925,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C94" s="14">
         <v>132</v>
@@ -12912,7 +12936,7 @@
         <v xml:space="preserve">DSS F.132 </v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="G94" s="7"/>
       <c r="H94" s="15"/>
@@ -12920,7 +12944,7 @@
       <c r="J94" s="7"/>
       <c r="K94" s="15"/>
       <c r="L94" s="15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="M94" s="15"/>
       <c r="N94" s="15"/>
@@ -12928,17 +12952,17 @@
         <v>33</v>
       </c>
       <c r="P94" s="15" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="Q94" s="7"/>
       <c r="R94" s="15"/>
       <c r="S94" s="15"/>
       <c r="T94" s="21"/>
       <c r="U94" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V94" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="95" spans="1:22" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12946,13 +12970,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C95" s="14">
         <v>168</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E95" s="10" t="str">
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
@@ -12960,7 +12984,7 @@
       </c>
       <c r="F95" s="7"/>
       <c r="G95" s="7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="H95" s="15" t="s">
         <v>135</v>
@@ -12977,19 +13001,19 @@
         <v>98</v>
       </c>
       <c r="P95" s="15" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="Q95" s="7"/>
       <c r="R95" s="15"/>
       <c r="S95" s="15"/>
       <c r="T95" s="21" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="U95" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V95" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="96" spans="1:22" ht="56" x14ac:dyDescent="0.2">
@@ -12997,7 +13021,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C96" s="14"/>
       <c r="D96" s="15"/>
@@ -13006,35 +13030,35 @@
         <v>Unidentified</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
       <c r="H96" s="15"/>
       <c r="I96" s="15"/>
       <c r="J96" s="7"/>
       <c r="K96" s="15"/>
       <c r="L96" s="15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="M96" s="15"/>
       <c r="N96" s="15"/>
       <c r="O96" s="15" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="P96" s="15" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="Q96" s="7"/>
       <c r="R96" s="15"/>
       <c r="S96" s="15"/>
       <c r="T96" s="21"/>
       <c r="U96" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V96" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="97" spans="1:22" ht="126" x14ac:dyDescent="0.2">
@@ -13042,7 +13066,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C97" s="14"/>
       <c r="D97" s="15"/>
@@ -13052,14 +13076,14 @@
       </c>
       <c r="F97" s="7"/>
       <c r="G97" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H97" s="15"/>
       <c r="I97" s="15"/>
       <c r="J97" s="7"/>
       <c r="K97" s="15"/>
       <c r="L97" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
@@ -13070,10 +13094,10 @@
       <c r="S97" s="15"/>
       <c r="T97" s="21"/>
       <c r="U97" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V97" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="98" spans="1:22" ht="126" x14ac:dyDescent="0.2">
@@ -13081,7 +13105,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C98" s="14"/>
       <c r="D98" s="15"/>
@@ -13091,14 +13115,14 @@
       </c>
       <c r="F98" s="7"/>
       <c r="G98" s="7" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="H98" s="15"/>
       <c r="I98" s="15"/>
       <c r="J98" s="7"/>
       <c r="K98" s="15"/>
       <c r="L98" s="15" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="M98" s="15"/>
       <c r="N98" s="15"/>
@@ -13109,10 +13133,10 @@
       <c r="S98" s="15"/>
       <c r="T98" s="21"/>
       <c r="U98" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V98" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="99" spans="1:22" ht="45" x14ac:dyDescent="0.2">
@@ -13120,7 +13144,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C99" s="14"/>
       <c r="D99" s="15"/>
@@ -13129,7 +13153,7 @@
         <v>Unidentified</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="G99" s="7"/>
       <c r="H99" s="15"/>
@@ -13137,7 +13161,7 @@
       <c r="J99" s="7"/>
       <c r="K99" s="15"/>
       <c r="L99" s="15" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="M99" s="15"/>
       <c r="N99" s="15"/>
@@ -13148,10 +13172,10 @@
       <c r="S99" s="15"/>
       <c r="T99" s="21"/>
       <c r="U99" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V99" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="100" spans="1:22" ht="45" x14ac:dyDescent="0.2">
@@ -13159,7 +13183,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C100" s="14"/>
       <c r="D100" s="15"/>
@@ -13168,7 +13192,7 @@
         <v>Unidentified</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="G100" s="7"/>
       <c r="H100" s="15"/>
@@ -13176,7 +13200,7 @@
       <c r="J100" s="7"/>
       <c r="K100" s="15"/>
       <c r="L100" s="15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="M100" s="15"/>
       <c r="N100" s="15"/>
@@ -13187,10 +13211,10 @@
       <c r="S100" s="15"/>
       <c r="T100" s="21"/>
       <c r="U100" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V100" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="101" spans="1:22" ht="45" x14ac:dyDescent="0.2">
@@ -13198,7 +13222,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="15" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C101" s="14"/>
       <c r="D101" s="15"/>
@@ -13207,7 +13231,7 @@
         <v>Unidentified</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="G101" s="7"/>
       <c r="H101" s="15"/>
@@ -13215,7 +13239,7 @@
       <c r="J101" s="7"/>
       <c r="K101" s="15"/>
       <c r="L101" s="15" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="M101" s="15"/>
       <c r="N101" s="15"/>
@@ -13226,18 +13250,18 @@
       <c r="S101" s="15"/>
       <c r="T101" s="21"/>
       <c r="U101" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V101" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="102" spans="1:22" ht="45" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B102" s="15" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C102" s="14"/>
       <c r="D102" s="15"/>
@@ -13247,17 +13271,17 @@
       </c>
       <c r="F102" s="7"/>
       <c r="G102" s="7" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="H102" s="15"/>
       <c r="I102" s="15"/>
       <c r="J102" s="7"/>
       <c r="K102" s="15"/>
       <c r="L102" s="15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="M102" s="15" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="N102" s="15"/>
       <c r="O102" s="15"/>
@@ -13267,10 +13291,10 @@
       <c r="S102" s="15"/>
       <c r="T102" s="21"/>
       <c r="U102" s="15" t="s">
-        <v>596</v>
+        <v>625</v>
       </c>
       <c r="V102" s="1" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed position of col. Current Owner
</commit_message>
<xml_diff>
--- a/data/post2002DB-v2.xlsx
+++ b/data/post2002DB-v2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hildad/Documents/GitHub/lyingpendatabases/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3513BAE4-9CAA-5542-9489-18C37414B4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B35830-4197-F442-BC53-F8FED5FE25C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{CB7DAB00-11D3-3A4F-BDDA-5DEC01C2CC59}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{CB7DAB00-11D3-3A4F-BDDA-5DEC01C2CC59}"/>
   </bookViews>
   <sheets>
     <sheet name="Database of Post-2002 Fragments" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_GoBack" localSheetId="0">'Database of Post-2002 Fragments'!$G$10</definedName>
+    <definedName name="_GoBack" localSheetId="0">'Database of Post-2002 Fragments'!$H$10</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -94,7 +94,7 @@
     Har jeg eller du den?</t>
       </text>
     </comment>
-    <comment ref="H8" authorId="4" shapeId="0" xr:uid="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
+    <comment ref="I8" authorId="4" shapeId="0" xr:uid="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -104,7 +104,7 @@
     Ja. Det bør inn :)</t>
       </text>
     </comment>
-    <comment ref="I8" authorId="5" shapeId="0" xr:uid="{6D446EEB-A84E-1D4E-9690-7BBD845E700E}">
+    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{6D446EEB-A84E-1D4E-9690-7BBD845E700E}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,7 +128,7 @@
     Kilde </t>
       </text>
     </comment>
-    <comment ref="I10" authorId="8" shapeId="0" xr:uid="{31C85DC9-8535-E64A-9D2C-8875E7AA0864}">
+    <comment ref="J10" authorId="8" shapeId="0" xr:uid="{31C85DC9-8535-E64A-9D2C-8875E7AA0864}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -168,7 +168,7 @@
     Er NOVA-referansen riktig?</t>
       </text>
     </comment>
-    <comment ref="H80" authorId="13" shapeId="0" xr:uid="{2DF247D5-F5AB-0F43-BB23-04B9F21B7B37}">
+    <comment ref="I80" authorId="13" shapeId="0" xr:uid="{2DF247D5-F5AB-0F43-BB23-04B9F21B7B37}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -197,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="623">
   <si>
     <t>No.</t>
   </si>
@@ -6812,6 +6812,15 @@
   </si>
   <si>
     <t>Bibliography</t>
+  </si>
+  <si>
+    <t>Museum of the Bible</t>
+  </si>
+  <si>
+    <t>Schøyen Collection</t>
+  </si>
+  <si>
+    <t>Azusa Pacific University</t>
   </si>
 </sst>
 </file>
@@ -7109,7 +7118,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color theme="0"/>
         <name val="Aleo Light"/>
         <scheme val="none"/>
       </font>
@@ -7146,6 +7155,488 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo Light"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Aleo"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -7193,300 +7684,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="8"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
         <sz val="10"/>
         <color theme="1"/>
         <name val="Aleo Light"/>
@@ -7530,7 +7727,7 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right/>
@@ -7553,18 +7750,19 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Aleo Light"/>
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top style="thin">
@@ -7573,197 +7771,8 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Aleo Light"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -7860,29 +7869,29 @@
   </sortState>
   <tableColumns count="23">
     <tableColumn id="1" xr3:uid="{4EFD41BC-5BFD-4E46-A5F1-7E906C6102C5}" name="No." dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{F93B8E3F-E2A9-9C46-8798-E2857A037AA3}" name="Content" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{4DDC7D22-B286-AD43-9DF0-FC7A4BACEAA9}" name="DSS F. No." dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{46E1AC7F-0FC2-3041-B3E2-F0809B37FB08}" name="DSS F. Name" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{AE8ADACF-00B6-7649-B9A0-10958EB147C4}" name="Name" dataDxfId="2">
+    <tableColumn id="15" xr3:uid="{F93B8E3F-E2A9-9C46-8798-E2857A037AA3}" name="Content" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{4DDC7D22-B286-AD43-9DF0-FC7A4BACEAA9}" name="DSS F. No." dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{46E1AC7F-0FC2-3041-B3E2-F0809B37FB08}" name="DSS F. Name" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{AE8ADACF-00B6-7649-B9A0-10958EB147C4}" name="Name" dataDxfId="18">
       <calculatedColumnFormula>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{142CBA6D-F3C5-874F-9A10-B4D0D370D4AD}" name="Collection No." dataDxfId="19"/>
-    <tableColumn id="32" xr3:uid="{9E02593A-E84E-124C-84CB-F3EC28D64481}" name="Name or Description" dataDxfId="18"/>
-    <tableColumn id="35" xr3:uid="{C459176B-7CFF-7741-81F6-696F6DDA7AC2}" name="Alleged Provenance" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{11BD8FB7-E8BA-EE49-B0FE-64041D98EB57}" name="False Identifications" dataDxfId="16"/>
-    <tableColumn id="28" xr3:uid="{7CFA9B31-34B3-1249-944A-FE370EC2B25E}" name="Siglum (Name) in Tov, Revised Lists (2010)" dataDxfId="15"/>
-    <tableColumn id="29" xr3:uid="{F6F3730C-3E78-9640-BD99-2AABB1F5151F}" name="Siglum and Fragment Number in Accordance" dataDxfId="14"/>
     <tableColumn id="19" xr3:uid="{F6AC96E7-4BB0-A14A-9245-5E3480975FD9}" name="Current Owner" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{E85C9271-D71B-2347-AC6C-CB969F40EC18}" name="Sale (➤), Donation (➢), and Collaboration (→)" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{B3E9F172-B29F-F14F-9417-580D64DFAF47}" name="Asking Price" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{91E1017E-7A63-B64C-B629-BFE8CFEC540C}" name="Purchase Price_x000a_Dealer/Seller ➤ Collector/Buyer" dataDxfId="11"/>
-    <tableColumn id="9" xr3:uid="{652C307D-EFC9-A44D-B6B7-7E5415A0E08F}" name="Lines" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{0B1022CB-F629-D54B-ACE5-24014EED6254}" name="Measurements_x000a_(in cm)" dataDxfId="9"/>
-    <tableColumn id="12" xr3:uid="{4665D607-2EED-974F-8F27-60FF09978FC3}" name="First Edition" dataDxfId="8"/>
-    <tableColumn id="30" xr3:uid="{AA398F82-26DF-A14A-BFA3-776AC4A147A7}" name="Edition 2" dataDxfId="7"/>
-    <tableColumn id="33" xr3:uid="{147BF4CF-F264-6B48-AC69-D7AEB150B2A1}" name="Frg. Part of a Ms Edition" dataDxfId="6"/>
-    <tableColumn id="34" xr3:uid="{516E9851-23BA-4E51-9FAE-45E15B80C08C}" name="Bibliography" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{BA6B59E9-7DD8-3F41-B53D-D836BA825549}" name="Content group" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{142CBA6D-F3C5-874F-9A10-B4D0D370D4AD}" name="Collection No." dataDxfId="17"/>
+    <tableColumn id="32" xr3:uid="{9E02593A-E84E-124C-84CB-F3EC28D64481}" name="Name or Description" dataDxfId="16"/>
+    <tableColumn id="35" xr3:uid="{C459176B-7CFF-7741-81F6-696F6DDA7AC2}" name="Alleged Provenance" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{11BD8FB7-E8BA-EE49-B0FE-64041D98EB57}" name="False Identifications" dataDxfId="14"/>
+    <tableColumn id="28" xr3:uid="{7CFA9B31-34B3-1249-944A-FE370EC2B25E}" name="Siglum (Name) in Tov, Revised Lists (2010)" dataDxfId="13"/>
+    <tableColumn id="29" xr3:uid="{F6F3730C-3E78-9640-BD99-2AABB1F5151F}" name="Siglum and Fragment Number in Accordance" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{E85C9271-D71B-2347-AC6C-CB969F40EC18}" name="Sale (➤), Donation (➢), and Collaboration (→)" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{B3E9F172-B29F-F14F-9417-580D64DFAF47}" name="Asking Price" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{91E1017E-7A63-B64C-B629-BFE8CFEC540C}" name="Purchase Price_x000a_Dealer/Seller ➤ Collector/Buyer" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{652C307D-EFC9-A44D-B6B7-7E5415A0E08F}" name="Lines" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{0B1022CB-F629-D54B-ACE5-24014EED6254}" name="Measurements_x000a_(in cm)" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{4665D607-2EED-974F-8F27-60FF09978FC3}" name="First Edition" dataDxfId="6"/>
+    <tableColumn id="30" xr3:uid="{AA398F82-26DF-A14A-BFA3-776AC4A147A7}" name="Edition 2" dataDxfId="5"/>
+    <tableColumn id="33" xr3:uid="{147BF4CF-F264-6B48-AC69-D7AEB150B2A1}" name="Frg. Part of a Ms Edition" dataDxfId="4"/>
+    <tableColumn id="34" xr3:uid="{516E9851-23BA-4E51-9FAE-45E15B80C08C}" name="Bibliography" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{BA6B59E9-7DD8-3F41-B53D-D836BA825549}" name="Content group" dataDxfId="2"/>
     <tableColumn id="17" xr3:uid="{9B268625-BF17-7245-969F-CCAF877DBC86}" name="Canonical group" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -8204,13 +8213,13 @@
   <threadedComment ref="U4" dT="2022-03-22T07:53:41.44" personId="{796E7543-8504-405A-8D6B-3A3CDE0CC86F}" id="{E2951F1D-27B5-461F-B0A9-FDE00BE0715F}" parentId="{32913907-D534-014C-A2B7-E0958F6ED919}">
     <text>Har jeg eller du den?</text>
   </threadedComment>
-  <threadedComment ref="H8" dT="2021-02-20T20:26:59.56" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
+  <threadedComment ref="I8" dT="2021-02-20T20:26:59.56" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
     <text xml:space="preserve">Ludvik, vi må vurdere om vi skal ta inn Fields’ røverhistorier fra YouTube-forelesningen sin. </text>
   </threadedComment>
-  <threadedComment ref="H8" dT="2021-02-26T15:28:02.79" personId="{796E7543-8504-405A-8D6B-3A3CDE0CC86F}" id="{471E5202-2BFC-41DC-A843-8872D836EE22}" parentId="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
+  <threadedComment ref="I8" dT="2021-02-26T15:28:02.79" personId="{796E7543-8504-405A-8D6B-3A3CDE0CC86F}" id="{471E5202-2BFC-41DC-A843-8872D836EE22}" parentId="{063009AE-1C47-5A44-9964-20755F5B4EFA}">
     <text>Ja. Det bør inn :)</text>
   </threadedComment>
-  <threadedComment ref="I8" dT="2021-03-02T20:18:22.58" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{6D446EEB-A84E-1D4E-9690-7BBD845E700E}">
+  <threadedComment ref="J8" dT="2021-03-02T20:18:22.58" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{6D446EEB-A84E-1D4E-9690-7BBD845E700E}">
     <text xml:space="preserve">Dette tror jeg at jeg har fra et privat dokument fra Fields til Schøyen. Bør nok ut før vi publiserer. </text>
   </threadedComment>
   <threadedComment ref="N8" dT="2021-02-19T09:08:31.88" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{B44D4F9E-62F4-CD4B-9A98-270C94C38314}">
@@ -8219,7 +8228,7 @@
   <threadedComment ref="Q8" dT="2021-02-19T09:10:29.32" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{6E557DC4-AD42-5247-8DD6-3E02255DDE54}">
     <text xml:space="preserve">Kilde </text>
   </threadedComment>
-  <threadedComment ref="I10" dT="2021-02-19T09:26:50.87" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{31C85DC9-8535-E64A-9D2C-8875E7AA0864}">
+  <threadedComment ref="J10" dT="2021-02-19T09:26:50.87" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{31C85DC9-8535-E64A-9D2C-8875E7AA0864}">
     <text>Sjekk lange</text>
   </threadedComment>
   <threadedComment ref="U10" dT="2021-04-19T09:22:50.36" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{821C7E93-B4E4-1847-850F-757E6089B046}">
@@ -8234,7 +8243,7 @@
   <threadedComment ref="U78" dT="2022-03-22T07:03:48.73" personId="{8876FAA3-BF0D-9247-B3AB-636F8762BE46}" id="{F37999FA-2FA5-1648-A58C-71FF2FEE16A1}">
     <text>Er NOVA-referansen riktig?</text>
   </threadedComment>
-  <threadedComment ref="H80" dT="2022-03-22T16:47:12.52" personId="{8876FAA3-BF0D-9247-B3AB-636F8762BE46}" id="{2DF247D5-F5AB-0F43-BB23-04B9F21B7B37}">
+  <threadedComment ref="I80" dT="2022-03-22T16:47:12.52" personId="{8876FAA3-BF0D-9247-B3AB-636F8762BE46}" id="{2DF247D5-F5AB-0F43-BB23-04B9F21B7B37}">
     <text>Legg inn quotes fra Tovs artikkel</text>
   </threadedComment>
   <threadedComment ref="U90" dT="2021-03-02T11:52:46.61" personId="{B27B2B84-CF82-ED4C-9691-AFC35911EFDC}" id="{F55427C9-A137-474F-BE0B-CB9064F94C63}">
@@ -8250,9 +8259,9 @@
   </sheetPr>
   <dimension ref="A1:W102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="220" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U86" sqref="U86"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="119" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F102" sqref="F102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8262,35 +8271,38 @@
     <col min="3" max="3" width="15.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="30" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.59765625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="29.59765625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="52.3984375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="43.796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.19921875" style="1" customWidth="1"/>
-    <col min="11" max="12" width="31.796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="65.3984375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="15.3984375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="54.59765625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.19921875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="25" style="1" customWidth="1"/>
-    <col min="19" max="19" width="30.3984375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="65.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="94" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="65.59765625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="35.59765625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="38.796875" style="1" customWidth="1"/>
-    <col min="26" max="26" width="30" style="1" customWidth="1"/>
-    <col min="27" max="27" width="32.3984375" style="1" customWidth="1"/>
-    <col min="28" max="28" width="31.3984375" style="1" customWidth="1"/>
-    <col min="29" max="29" width="31.19921875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="28" style="1" customWidth="1"/>
-    <col min="31" max="31" width="37" style="1" customWidth="1"/>
-    <col min="32" max="32" width="40" style="1" customWidth="1"/>
-    <col min="33" max="33" width="30.3984375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="40.19921875" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="11" style="1"/>
+    <col min="6" max="6" width="31.796875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.59765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="52.3984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.796875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
+    <col min="12" max="12" width="37.19921875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="64" style="1" customWidth="1"/>
+    <col min="14" max="14" width="25.19921875" customWidth="1"/>
+    <col min="15" max="15" width="65.3984375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.3984375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="54.59765625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.19921875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="25" style="1" customWidth="1"/>
+    <col min="21" max="21" width="30.3984375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="40.796875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="94" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="65.59765625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="35.59765625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="38.796875" style="1" customWidth="1"/>
+    <col min="28" max="28" width="30" style="1" customWidth="1"/>
+    <col min="29" max="29" width="32.3984375" style="1" customWidth="1"/>
+    <col min="30" max="30" width="31.3984375" style="1" customWidth="1"/>
+    <col min="31" max="31" width="31.19921875" style="1" customWidth="1"/>
+    <col min="32" max="32" width="28" style="1" customWidth="1"/>
+    <col min="33" max="33" width="37" style="1" customWidth="1"/>
+    <col min="34" max="34" width="40" style="1" customWidth="1"/>
+    <col min="35" max="35" width="30.3984375" style="1" customWidth="1"/>
+    <col min="36" max="36" width="40.19921875" style="1" customWidth="1"/>
+    <col min="37" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="73" customHeight="1" x14ac:dyDescent="0.2">
@@ -8310,25 +8322,25 @@
         <v>1</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>520</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>550</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>594</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>576</v>
@@ -8377,21 +8389,21 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Gen 13:1–3</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="6"/>
+      <c r="I2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="13"/>
       <c r="M2" s="12" t="s">
         <v>17</v>
       </c>
@@ -8420,7 +8432,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="370" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -8433,25 +8445,25 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Words from Genesis 22</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="15"/>
+      <c r="G3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="J3" s="15" t="s">
         <v>545</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="15"/>
       <c r="M3" s="15" t="s">
         <v>609</v>
       </c>
@@ -8503,16 +8515,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.191 Gen2</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="25" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="25" t="s">
         <v>509</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="7"/>
       <c r="L4" s="15"/>
       <c r="M4" s="15" t="s">
         <v>577</v>
@@ -8540,7 +8554,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="83" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23" ht="183" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -8553,22 +8567,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Gen 33:19–34:2</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="M5" s="15"/>
       <c r="N5" s="15"/>
       <c r="O5" s="15"/>
       <c r="P5" s="15" t="s">
@@ -8609,18 +8623,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.101 Gen1</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="7"/>
       <c r="L6" s="15"/>
       <c r="M6" s="15" t="s">
         <v>52</v>
@@ -8667,18 +8683,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.102 RP1</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="7"/>
+      <c r="I7" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="J7" s="15" t="s">
         <v>546</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7" s="17"/>
+      <c r="K7" s="23"/>
       <c r="L7" s="17"/>
       <c r="M7" s="15" t="s">
         <v>62</v>
@@ -8708,7 +8726,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="135" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23" ht="210" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -8721,22 +8739,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Gen 37:26–38</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="J8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="15"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="15"/>
-      <c r="M8" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="M8" s="15"/>
       <c r="N8" s="15" t="s">
         <v>602</v>
       </c>
@@ -8760,7 +8778,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -8773,16 +8791,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Gen 47:4–5</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="15"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="15"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="15"/>
-      <c r="M9" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="M9" s="15"/>
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
@@ -8817,23 +8835,25 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.103 Exod3</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="15" t="s">
+      <c r="H10" s="7"/>
+      <c r="I10" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="J10" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="K10" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K10" s="15" t="s">
+      <c r="L10" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="L10" s="15"/>
       <c r="M10" s="15" t="s">
         <v>84</v>
       </c>
@@ -8875,23 +8895,25 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.104 Exod4</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="G11" s="7"/>
-      <c r="H11" s="15" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="J11" s="15" t="s">
         <v>547</v>
       </c>
-      <c r="J11" s="7" t="s">
+      <c r="K11" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="L11" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="L11" s="15"/>
       <c r="M11" s="15" t="s">
         <v>84</v>
       </c>
@@ -8916,7 +8938,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -8929,16 +8951,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Exod 6:11–12, 26–29</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G12" s="7"/>
-      <c r="H12" s="15"/>
+      <c r="H12" s="7"/>
       <c r="I12" s="15"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="15"/>
-      <c r="M12" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="M12" s="15"/>
       <c r="N12" s="15"/>
       <c r="O12" s="15"/>
       <c r="P12" s="15"/>
@@ -8956,7 +8978,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" ht="160" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -8969,14 +8991,14 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Exod 12:3–5</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="15" t="s">
+      <c r="H13" s="7"/>
+      <c r="I13" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="15"/>
       <c r="M13" s="15" t="s">
         <v>98</v>
@@ -9000,7 +9022,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -9013,16 +9035,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Exod 12:25–27</v>
       </c>
-      <c r="F14" s="7"/>
+      <c r="F14" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="15"/>
+      <c r="H14" s="7"/>
       <c r="I14" s="15"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="7"/>
       <c r="L14" s="15"/>
-      <c r="M14" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="M14" s="15"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
       <c r="P14" s="15"/>
@@ -9040,7 +9062,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="90" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" ht="110" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -9057,20 +9079,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.105 Exod5</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="7"/>
+      <c r="I15" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="I15" s="18" t="s">
+      <c r="J15" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="J15" s="7" t="s">
+      <c r="K15" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15" t="s">
         <v>84</v>
@@ -9113,16 +9137,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.192 Exod6</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="15"/>
+      <c r="H16" s="7"/>
       <c r="I16" s="15"/>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="15"/>
+      <c r="K16" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15" t="s">
         <v>578</v>
@@ -9165,18 +9191,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.151 (Unid) [earlier: DDS F.Exod1]</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="15" t="s">
+      <c r="H17" s="7"/>
+      <c r="I17" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="7" t="s">
+      <c r="J17" s="15"/>
+      <c r="K17" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="K17" s="15"/>
       <c r="L17" s="15"/>
       <c r="M17" s="15" t="s">
         <v>579</v>
@@ -9221,18 +9249,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.161 Exod2</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="I18" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="7" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="K18" s="15"/>
       <c r="L18" s="15"/>
       <c r="M18" s="15" t="s">
         <v>127</v>
@@ -9271,17 +9299,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Lev 1:2–5</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="15"/>
       <c r="I19" s="15"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J19" s="15"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="15"/>
       <c r="M19" s="15"/>
       <c r="N19" s="15"/>
       <c r="O19" s="15"/>
@@ -9315,16 +9343,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.152 Lev1</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="15"/>
+      <c r="H20" s="7"/>
       <c r="I20" s="15"/>
-      <c r="J20" s="7" t="s">
+      <c r="J20" s="15"/>
+      <c r="K20" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="K20" s="15"/>
       <c r="L20" s="15"/>
       <c r="M20" s="15" t="s">
         <v>579</v>
@@ -9350,7 +9380,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -9363,15 +9393,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Lev 16:16–20</v>
       </c>
-      <c r="F21" s="7"/>
+      <c r="F21" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="15"/>
+      <c r="H21" s="7"/>
       <c r="I21" s="15"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J21" s="15"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="15"/>
       <c r="M21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
@@ -9407,20 +9437,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.162 Lev2</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7" t="s">
+      <c r="F22" s="17"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="H22" s="15" t="s">
+      <c r="I22" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="J22" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="J22" s="7" t="s">
+      <c r="K22" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="K22" s="17"/>
       <c r="L22" s="17"/>
       <c r="M22" s="15" t="s">
         <v>127</v>
@@ -9450,7 +9480,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -9467,16 +9497,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.193 Lev5</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G23" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="15"/>
+      <c r="H23" s="7"/>
       <c r="I23" s="15"/>
-      <c r="J23" s="7" t="s">
+      <c r="J23" s="15"/>
+      <c r="K23" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="K23" s="15"/>
       <c r="L23" s="15"/>
       <c r="M23" s="15" t="s">
         <v>580</v>
@@ -9519,14 +9551,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.203 Lev6</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="15"/>
+      <c r="H24" s="7"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="7"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15" t="s">
         <v>581</v>
@@ -9550,7 +9584,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="25" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -9563,22 +9597,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Lev 23:38–39</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7" t="s">
+      <c r="F25" s="15" t="s">
+        <v>590</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="I25" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="7" t="s">
+      <c r="J25" s="15"/>
+      <c r="K25" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="L25" s="15" t="s">
         <v>158</v>
-      </c>
-      <c r="L25" s="15" t="s">
-        <v>590</v>
       </c>
       <c r="M25" s="15" t="s">
         <v>589</v>
@@ -9610,7 +9644,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -9623,22 +9657,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Lev 23:40–44, 24:16–19</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="15" t="s">
+        <v>590</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="H26" s="15" t="s">
+      <c r="I26" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="I26" s="15"/>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="15"/>
+      <c r="K26" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="L26" s="15" t="s">
         <v>165</v>
-      </c>
-      <c r="L26" s="15" t="s">
-        <v>590</v>
       </c>
       <c r="M26" s="15" t="s">
         <v>589</v>
@@ -9670,7 +9704,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="27" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -9683,19 +9717,19 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Cluster of miniscule pieces</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7" t="s">
+      <c r="F27" s="15" t="s">
+        <v>590</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="I27" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15" t="s">
-        <v>590</v>
-      </c>
+      <c r="J27" s="15"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="15"/>
       <c r="M27" s="15" t="s">
         <v>589</v>
       </c>
@@ -9722,7 +9756,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -9735,15 +9769,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Num 1:15–16</v>
       </c>
-      <c r="F28" s="7"/>
+      <c r="F28" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G28" s="7"/>
-      <c r="H28" s="15"/>
+      <c r="H28" s="7"/>
       <c r="I28" s="15"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J28" s="15"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="15"/>
       <c r="M28" s="15"/>
       <c r="N28" s="15"/>
       <c r="O28" s="15"/>
@@ -9762,7 +9796,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="29" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -9775,15 +9809,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Num 8:2–3</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="15"/>
+      <c r="H29" s="7"/>
       <c r="I29" s="15"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J29" s="15"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="15"/>
       <c r="M29" s="15"/>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
@@ -9802,7 +9836,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="30" spans="1:23" ht="40" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:23" ht="110" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -9819,14 +9853,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.194 Num2</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="15"/>
+      <c r="H30" s="7"/>
       <c r="I30" s="15"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="7"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15" t="s">
         <v>582</v>
@@ -9852,7 +9888,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -9865,15 +9901,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Num 8:15–17</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G31" s="7"/>
-      <c r="H31" s="15"/>
+      <c r="H31" s="7"/>
       <c r="I31" s="15"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J31" s="15"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="15"/>
       <c r="M31" s="15"/>
       <c r="N31" s="15"/>
       <c r="O31" s="15"/>
@@ -9909,20 +9945,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.107 Num1</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="H32" s="15" t="s">
+      <c r="I32" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="J32" s="15" t="s">
         <v>548</v>
       </c>
-      <c r="J32" s="7"/>
-      <c r="K32" s="15"/>
+      <c r="K32" s="7"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15" t="s">
         <v>52</v>
@@ -9950,7 +9988,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -9963,15 +10001,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Deut 4:47–5:5</v>
       </c>
-      <c r="F33" s="7"/>
+      <c r="F33" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G33" s="7"/>
-      <c r="H33" s="15"/>
+      <c r="H33" s="7"/>
       <c r="I33" s="15"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J33" s="15"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="15"/>
       <c r="M33" s="15"/>
       <c r="N33" s="15"/>
       <c r="O33" s="15"/>
@@ -9990,7 +10028,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -10007,20 +10045,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.108 Deut5</v>
       </c>
-      <c r="F34" s="7" t="s">
+      <c r="F34" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="G34" s="7" t="s">
+      <c r="H34" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="15"/>
+      <c r="J34" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="K34" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="K34" s="17"/>
       <c r="L34" s="17"/>
       <c r="M34" s="15" t="s">
         <v>192</v>
@@ -10048,7 +10088,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:23" ht="130" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -10065,16 +10105,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.153 Deut1</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="G35" s="7"/>
-      <c r="H35" s="15"/>
+      <c r="H35" s="7"/>
       <c r="I35" s="15"/>
-      <c r="J35" s="7" t="s">
+      <c r="J35" s="15"/>
+      <c r="K35" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="K35" s="15"/>
       <c r="L35" s="15"/>
       <c r="M35" s="15" t="s">
         <v>199</v>
@@ -10117,18 +10159,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.163 Deut3</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="17"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="15" t="s">
+      <c r="H36" s="7"/>
+      <c r="I36" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="J36" s="15" t="s">
         <v>515</v>
       </c>
-      <c r="J36" s="7" t="s">
+      <c r="K36" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="K36" s="17"/>
       <c r="L36" s="17"/>
       <c r="M36" s="15" t="s">
         <v>203</v>
@@ -10171,18 +10213,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.164 Deut4</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7" t="s">
+      <c r="F37" s="15"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="H37" s="15" t="s">
+      <c r="I37" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="7" t="s">
+      <c r="J37" s="15"/>
+      <c r="K37" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="K37" s="15"/>
       <c r="L37" s="15"/>
       <c r="M37" s="15" t="s">
         <v>203</v>
@@ -10208,7 +10250,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -10221,15 +10263,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Deut 16:1–3</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G38" s="7"/>
-      <c r="H38" s="15"/>
+      <c r="H38" s="7"/>
       <c r="I38" s="15"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J38" s="15"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="15"/>
       <c r="M38" s="15"/>
       <c r="N38" s="15"/>
       <c r="O38" s="15"/>
@@ -10262,21 +10304,21 @@
         <v>Deut 19:13–15 [Eshel and Eshel 2007]
 Deut 23:3–4 [Puech?; Charlesworth?]</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="15"/>
+      <c r="G39" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="G39" s="7"/>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15" t="s">
+      <c r="H39" s="7"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15" t="s">
         <v>552</v>
       </c>
-      <c r="J39" s="7" t="s">
+      <c r="K39" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="L39" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="L39" s="15"/>
       <c r="M39" s="15" t="s">
         <v>591</v>
       </c>
@@ -10322,18 +10364,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.154 Deut2</v>
       </c>
-      <c r="F40" s="7" t="s">
+      <c r="F40" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="G40" s="7" t="s">
+      <c r="H40" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="H40" s="15"/>
       <c r="I40" s="15"/>
-      <c r="J40" s="7" t="s">
+      <c r="J40" s="15"/>
+      <c r="K40" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15" t="s">
         <v>592</v>
@@ -10374,15 +10418,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Deut 31:12–13</v>
       </c>
-      <c r="F41" s="7"/>
+      <c r="F41" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G41" s="7"/>
-      <c r="H41" s="15"/>
+      <c r="H41" s="7"/>
       <c r="I41" s="15"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J41" s="15"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="15"/>
       <c r="M41" s="15"/>
       <c r="N41" s="15"/>
       <c r="O41" s="15"/>
@@ -10418,18 +10462,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.109 Deut6</v>
       </c>
-      <c r="F42" s="7" t="s">
+      <c r="F42" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="G42" s="7" t="s">
+      <c r="H42" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="H42" s="15" t="s">
+      <c r="I42" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="15"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="7"/>
       <c r="L42" s="15"/>
       <c r="M42" s="15" t="s">
         <v>52</v>
@@ -10457,7 +10503,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="43" spans="1:23" ht="50" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -10470,20 +10516,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Judg 1:10–12</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G43" s="7"/>
-      <c r="H43" s="15"/>
-      <c r="I43" s="15" t="s">
+      <c r="H43" s="7"/>
+      <c r="I43" s="15"/>
+      <c r="J43" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="K43" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="L43" s="15" t="s">
         <v>239</v>
-      </c>
-      <c r="L43" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="M43" s="15"/>
       <c r="N43" s="15"/>
@@ -10509,7 +10555,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="44" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:23" ht="70" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -10522,20 +10568,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Judg 4:6–8</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7" t="s">
+      <c r="F44" s="15" t="s">
+        <v>595</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="H44" s="15"/>
       <c r="I44" s="15"/>
-      <c r="J44" s="9" t="s">
+      <c r="J44" s="15"/>
+      <c r="K44" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="L44" s="15" t="s">
         <v>247</v>
-      </c>
-      <c r="L44" s="15" t="s">
-        <v>595</v>
       </c>
       <c r="M44" s="15"/>
       <c r="N44" s="15"/>
@@ -10561,7 +10607,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="45" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -10574,15 +10620,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Judg 8:3–6</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G45" s="7"/>
-      <c r="H45" s="15"/>
+      <c r="H45" s="7"/>
       <c r="I45" s="15"/>
-      <c r="J45" s="7"/>
-      <c r="K45" s="15"/>
-      <c r="L45" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J45" s="15"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="15"/>
       <c r="M45" s="15"/>
       <c r="N45" s="15"/>
       <c r="O45" s="15"/>
@@ -10601,7 +10647,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="46" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:23" ht="57" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -10614,17 +10660,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Judg 19:10–13, 23–28</v>
       </c>
-      <c r="F46" s="7"/>
+      <c r="F46" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G46" s="7"/>
-      <c r="H46" s="15"/>
+      <c r="H46" s="7"/>
       <c r="I46" s="15"/>
-      <c r="J46" s="7" t="s">
+      <c r="J46" s="15"/>
+      <c r="K46" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="L46" s="15"/>
       <c r="M46" s="15"/>
       <c r="N46" s="15"/>
       <c r="O46" s="15"/>
@@ -10662,16 +10708,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.120 Ruth1</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="H47" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="H47" s="15"/>
       <c r="I47" s="15"/>
-      <c r="J47" s="7"/>
-      <c r="K47" s="15"/>
+      <c r="J47" s="15"/>
+      <c r="K47" s="7"/>
       <c r="L47" s="15"/>
       <c r="M47" s="15" t="s">
         <v>260</v>
@@ -10716,14 +10764,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.112 Sam1</v>
       </c>
-      <c r="F48" s="7" t="s">
+      <c r="F48" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G48" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="G48" s="7"/>
-      <c r="H48" s="15"/>
+      <c r="H48" s="7"/>
       <c r="I48" s="15"/>
-      <c r="J48" s="7"/>
-      <c r="K48" s="15"/>
+      <c r="J48" s="15"/>
+      <c r="K48" s="7"/>
       <c r="L48" s="15"/>
       <c r="M48" s="15" t="s">
         <v>266</v>
@@ -10768,18 +10818,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.113 Sam2</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G49" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="H49" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="H49" s="15" t="s">
+      <c r="I49" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I49" s="15"/>
-      <c r="J49" s="7"/>
-      <c r="K49" s="15"/>
+      <c r="J49" s="15"/>
+      <c r="K49" s="7"/>
       <c r="L49" s="15"/>
       <c r="M49" s="15" t="s">
         <v>266</v>
@@ -10807,7 +10859,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>49</v>
       </c>
@@ -10820,15 +10872,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>2(?)Sam 5:10–12</v>
       </c>
-      <c r="F50" s="7"/>
+      <c r="F50" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G50" s="7"/>
-      <c r="H50" s="15"/>
+      <c r="H50" s="7"/>
       <c r="I50" s="15"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="15"/>
-      <c r="L50" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J50" s="15"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="15"/>
       <c r="M50" s="15"/>
       <c r="N50" s="15"/>
       <c r="O50" s="15"/>
@@ -10847,7 +10899,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>50</v>
       </c>
@@ -10864,20 +10916,22 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.114 Sam3</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G51" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="H51" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="H51" s="15"/>
-      <c r="I51" s="15" t="s">
+      <c r="I51" s="15"/>
+      <c r="J51" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="J51" s="7" t="s">
+      <c r="K51" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="K51" s="15"/>
       <c r="L51" s="15"/>
       <c r="M51" s="15" t="s">
         <v>192</v>
@@ -10905,7 +10959,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>51</v>
       </c>
@@ -10922,12 +10976,12 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.170 Kings</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="15"/>
       <c r="G52" s="7"/>
-      <c r="H52" s="15"/>
+      <c r="H52" s="7"/>
       <c r="I52" s="15"/>
-      <c r="J52" s="7"/>
-      <c r="K52" s="15"/>
+      <c r="J52" s="15"/>
+      <c r="K52" s="7"/>
       <c r="L52" s="15"/>
       <c r="M52" s="15" t="s">
         <v>286</v>
@@ -10970,18 +11024,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.115 Kgs1</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G53" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="G53" s="7" t="s">
+      <c r="H53" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="H53" s="15" t="s">
+      <c r="I53" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="7"/>
-      <c r="K53" s="15"/>
+      <c r="J53" s="15"/>
+      <c r="K53" s="7"/>
       <c r="L53" s="15"/>
       <c r="M53" s="15" t="s">
         <v>293</v>
@@ -11007,7 +11063,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="54" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>53</v>
       </c>
@@ -11020,15 +11076,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>1(?) Kgs 18:8–10</v>
       </c>
-      <c r="F54" s="7"/>
+      <c r="F54" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G54" s="7"/>
-      <c r="H54" s="15"/>
+      <c r="H54" s="7"/>
       <c r="I54" s="15"/>
-      <c r="J54" s="7"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J54" s="15"/>
+      <c r="K54" s="7"/>
+      <c r="L54" s="15"/>
       <c r="M54" s="15"/>
       <c r="N54" s="15"/>
       <c r="O54" s="15"/>
@@ -11060,15 +11116,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>2(?) Kgs 11:17–18</v>
       </c>
-      <c r="F55" s="7"/>
+      <c r="F55" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G55" s="7"/>
-      <c r="H55" s="15"/>
+      <c r="H55" s="7"/>
       <c r="I55" s="15"/>
-      <c r="J55" s="7"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J55" s="15"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="15"/>
       <c r="M55" s="15"/>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
@@ -11087,7 +11143,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="60" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:23" ht="160" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>55</v>
       </c>
@@ -11104,14 +11160,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.201 Neh2</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G56" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="15"/>
+      <c r="H56" s="7"/>
       <c r="I56" s="15"/>
-      <c r="J56" s="7"/>
-      <c r="K56" s="15"/>
+      <c r="J56" s="15"/>
+      <c r="K56" s="7"/>
       <c r="L56" s="15"/>
       <c r="M56" s="15" t="s">
         <v>582</v>
@@ -11154,18 +11212,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.122 Neh1</v>
       </c>
-      <c r="F57" s="7" t="s">
+      <c r="F57" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G57" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="G57" s="7"/>
-      <c r="H57" s="25" t="s">
+      <c r="H57" s="7"/>
+      <c r="I57" s="25" t="s">
         <v>516</v>
       </c>
-      <c r="I57" s="15"/>
-      <c r="J57" s="7" t="s">
+      <c r="J57" s="15"/>
+      <c r="K57" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="K57" s="15"/>
       <c r="L57" s="15"/>
       <c r="M57" s="15" t="s">
         <v>307</v>
@@ -11212,18 +11272,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.118 Ps2</v>
       </c>
-      <c r="F58" s="7" t="s">
+      <c r="F58" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G58" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="G58" s="7" t="s">
+      <c r="H58" s="7" t="s">
         <v>314</v>
       </c>
-      <c r="H58" s="15"/>
       <c r="I58" s="15"/>
-      <c r="J58" s="15" t="s">
+      <c r="J58" s="15"/>
+      <c r="K58" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="K58" s="15"/>
       <c r="L58" s="15"/>
       <c r="M58" s="15" t="s">
         <v>316</v>
@@ -11268,23 +11330,25 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.199 Ps3</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="19" t="s">
+        <v>620</v>
+      </c>
+      <c r="G59" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="H59" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="H59" s="15"/>
-      <c r="I59" s="19" t="s">
+      <c r="I59" s="15"/>
+      <c r="J59" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="J59" s="8" t="s">
+      <c r="K59" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="K59" s="19" t="s">
+      <c r="L59" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="L59" s="19"/>
       <c r="M59" s="15" t="s">
         <v>583</v>
       </c>
@@ -11326,21 +11390,21 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Ps 11:1–3</v>
       </c>
-      <c r="F60" s="7"/>
+      <c r="F60" s="15"/>
       <c r="G60" s="7"/>
-      <c r="H60" s="15" t="s">
+      <c r="H60" s="7"/>
+      <c r="I60" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="I60" s="15" t="s">
+      <c r="J60" s="15" t="s">
         <v>553</v>
       </c>
-      <c r="J60" s="8" t="s">
+      <c r="K60" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="K60" s="15" t="s">
+      <c r="L60" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="L60" s="15"/>
       <c r="M60" s="15" t="s">
         <v>334</v>
       </c>
@@ -11380,18 +11444,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.165 Ps1</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7" t="s">
+      <c r="F61" s="15"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="H61" s="15" t="s">
+      <c r="I61" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I61" s="15" t="s">
+      <c r="J61" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="J61" s="7"/>
-      <c r="K61" s="15"/>
+      <c r="K61" s="7"/>
       <c r="L61" s="15"/>
       <c r="M61" s="15" t="s">
         <v>551</v>
@@ -11417,7 +11481,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>61</v>
       </c>
@@ -11430,15 +11494,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Ps 119:17, 28</v>
       </c>
-      <c r="F62" s="7"/>
+      <c r="F62" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G62" s="7"/>
-      <c r="H62" s="15"/>
+      <c r="H62" s="7"/>
       <c r="I62" s="15"/>
-      <c r="J62" s="7"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J62" s="15"/>
+      <c r="K62" s="7"/>
+      <c r="L62" s="15"/>
       <c r="M62" s="15"/>
       <c r="N62" s="15"/>
       <c r="O62" s="15"/>
@@ -11457,7 +11521,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="45" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:23" ht="90" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>62</v>
       </c>
@@ -11470,17 +11534,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Ps 119:40–44</v>
       </c>
-      <c r="F63" s="7"/>
+      <c r="F63" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G63" s="7"/>
-      <c r="H63" s="15" t="s">
+      <c r="H63" s="7"/>
+      <c r="I63" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="I63" s="15"/>
-      <c r="J63" s="7"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J63" s="15"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="15"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
       <c r="O63" s="15"/>
@@ -11512,15 +11576,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Ps 119:61–64</v>
       </c>
-      <c r="F64" s="7"/>
+      <c r="F64" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G64" s="7"/>
-      <c r="H64" s="15"/>
+      <c r="H64" s="7"/>
       <c r="I64" s="15"/>
-      <c r="J64" s="7"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J64" s="15"/>
+      <c r="K64" s="7"/>
+      <c r="L64" s="15"/>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
       <c r="O64" s="15"/>
@@ -11539,7 +11603,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="65" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>64</v>
       </c>
@@ -11556,16 +11620,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.119 Prov1</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G65" s="7" t="s">
         <v>349</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="H65" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="H65" s="15"/>
       <c r="I65" s="15"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="15"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="7"/>
       <c r="L65" s="15"/>
       <c r="M65" s="15" t="s">
         <v>52</v>
@@ -11604,23 +11670,23 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Isa 24:16–17</v>
       </c>
-      <c r="F66" s="7" t="s">
+      <c r="F66" s="15"/>
+      <c r="G66" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="G66" s="7"/>
-      <c r="H66" s="16" t="s">
+      <c r="H66" s="7"/>
+      <c r="I66" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I66" s="15" t="s">
+      <c r="J66" s="15" t="s">
         <v>554</v>
       </c>
-      <c r="J66" s="7" t="s">
+      <c r="K66" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="K66" s="15" t="s">
+      <c r="L66" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="L66" s="15"/>
       <c r="M66" s="15" t="s">
         <v>591</v>
       </c>
@@ -11651,7 +11717,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="67" spans="1:23" ht="153" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>66</v>
       </c>
@@ -11664,23 +11730,23 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Isa 26:19–27:1</v>
       </c>
-      <c r="F67" s="7" t="s">
+      <c r="F67" s="15"/>
+      <c r="G67" s="7" t="s">
         <v>361</v>
       </c>
-      <c r="G67" s="7"/>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="7"/>
+      <c r="I67" s="16" t="s">
         <v>362</v>
       </c>
-      <c r="I67" s="15" t="s">
+      <c r="J67" s="15" t="s">
         <v>555</v>
       </c>
-      <c r="J67" s="7" t="s">
+      <c r="K67" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="K67" s="15" t="s">
+      <c r="L67" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="L67" s="15"/>
       <c r="M67" s="15" t="s">
         <v>591</v>
       </c>
@@ -11724,17 +11790,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Isa 28:23–29</v>
       </c>
-      <c r="F68" s="7"/>
+      <c r="F68" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G68" s="7"/>
-      <c r="H68" s="15" t="s">
+      <c r="H68" s="7"/>
+      <c r="I68" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="I68" s="15"/>
-      <c r="J68" s="7"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J68" s="15"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="15"/>
       <c r="M68" s="15"/>
       <c r="N68" s="15"/>
       <c r="O68" s="15"/>
@@ -11757,7 +11823,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="69" spans="1:23" ht="165" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:23" ht="290" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>68</v>
       </c>
@@ -11774,22 +11840,24 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.116 Jer1</v>
       </c>
-      <c r="F69" s="7" t="s">
+      <c r="F69" s="17" t="s">
+        <v>621</v>
+      </c>
+      <c r="G69" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>373</v>
       </c>
-      <c r="H69" s="15" t="s">
+      <c r="I69" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="I69" s="15" t="s">
+      <c r="J69" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="J69" s="7" t="s">
+      <c r="K69" s="7" t="s">
         <v>375</v>
       </c>
-      <c r="K69" s="17"/>
       <c r="L69" s="17"/>
       <c r="M69" s="15" t="s">
         <v>52</v>
@@ -11817,7 +11885,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="70" spans="1:23" ht="80" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:23" ht="236" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>69</v>
       </c>
@@ -11834,14 +11902,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.195 Jer2</v>
       </c>
-      <c r="F70" s="7" t="s">
+      <c r="F70" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G70" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="G70" s="7"/>
-      <c r="H70" s="15"/>
+      <c r="H70" s="7"/>
       <c r="I70" s="15"/>
-      <c r="J70" s="7"/>
-      <c r="K70" s="15"/>
+      <c r="J70" s="15"/>
+      <c r="K70" s="7"/>
       <c r="L70" s="15"/>
       <c r="M70" s="15" t="s">
         <v>584</v>
@@ -11886,21 +11956,21 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.156 Jer3</v>
       </c>
-      <c r="F71" s="7"/>
+      <c r="F71" s="15"/>
       <c r="G71" s="7"/>
-      <c r="H71" s="15" t="s">
+      <c r="H71" s="7"/>
+      <c r="I71" s="15" t="s">
         <v>385</v>
       </c>
-      <c r="I71" s="15" t="s">
+      <c r="J71" s="15" t="s">
         <v>556</v>
       </c>
-      <c r="J71" s="7" t="s">
+      <c r="K71" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="K71" s="15" t="s">
+      <c r="L71" s="15" t="s">
         <v>387</v>
       </c>
-      <c r="L71" s="15"/>
       <c r="M71" s="15" t="s">
         <v>596</v>
       </c>
@@ -11927,7 +11997,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="72" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:23" ht="70" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>71</v>
       </c>
@@ -11944,14 +12014,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.196 Ezek1</v>
       </c>
-      <c r="F72" s="7" t="s">
+      <c r="F72" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G72" s="7" t="s">
         <v>392</v>
       </c>
-      <c r="G72" s="7"/>
-      <c r="H72" s="15"/>
+      <c r="H72" s="7"/>
       <c r="I72" s="15"/>
-      <c r="J72" s="7"/>
-      <c r="K72" s="15"/>
+      <c r="J72" s="15"/>
+      <c r="K72" s="7"/>
       <c r="L72" s="15"/>
       <c r="M72" s="15" t="s">
         <v>585</v>
@@ -11994,18 +12066,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.155 Dan1</v>
       </c>
-      <c r="F73" s="7" t="s">
+      <c r="F73" s="15" t="s">
+        <v>622</v>
+      </c>
+      <c r="G73" s="7" t="s">
         <v>397</v>
       </c>
-      <c r="G73" s="7"/>
-      <c r="H73" s="15" t="s">
+      <c r="H73" s="7"/>
+      <c r="I73" s="15" t="s">
         <v>398</v>
       </c>
-      <c r="I73" s="15"/>
-      <c r="J73" s="7" t="s">
+      <c r="J73" s="15"/>
+      <c r="K73" s="7" t="s">
         <v>399</v>
       </c>
-      <c r="K73" s="15"/>
       <c r="L73" s="15"/>
       <c r="M73" s="15" t="s">
         <v>579</v>
@@ -12050,18 +12124,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.166 Dan2</v>
       </c>
-      <c r="F74" s="7"/>
+      <c r="F74" s="15"/>
       <c r="G74" s="7"/>
-      <c r="H74" s="15" t="s">
+      <c r="H74" s="7"/>
+      <c r="I74" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I74" s="15" t="s">
+      <c r="J74" s="15" t="s">
         <v>403</v>
       </c>
-      <c r="J74" s="7" t="s">
+      <c r="K74" s="7" t="s">
         <v>404</v>
       </c>
-      <c r="K74" s="15"/>
       <c r="L74" s="15"/>
       <c r="M74" s="15" t="s">
         <v>127</v>
@@ -12104,14 +12178,14 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.167 Dan3</v>
       </c>
-      <c r="F75" s="7"/>
+      <c r="F75" s="15"/>
       <c r="G75" s="7"/>
-      <c r="H75" s="15" t="s">
+      <c r="H75" s="7"/>
+      <c r="I75" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I75" s="15"/>
-      <c r="J75" s="7"/>
-      <c r="K75" s="15"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="7"/>
       <c r="L75" s="15"/>
       <c r="M75" s="15" t="s">
         <v>127</v>
@@ -12137,7 +12211,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="76" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:23" ht="70" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>75</v>
       </c>
@@ -12154,14 +12228,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.200 Dan6</v>
       </c>
-      <c r="F76" s="7" t="s">
+      <c r="F76" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G76" s="7" t="s">
         <v>413</v>
       </c>
-      <c r="G76" s="7"/>
-      <c r="H76" s="15"/>
+      <c r="H76" s="7"/>
       <c r="I76" s="15"/>
-      <c r="J76" s="7"/>
-      <c r="K76" s="15"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="7"/>
       <c r="L76" s="15"/>
       <c r="M76" s="15" t="s">
         <v>585</v>
@@ -12187,7 +12263,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="77" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>76</v>
       </c>
@@ -12200,15 +12276,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Joel 2:23–26</v>
       </c>
-      <c r="F77" s="7"/>
+      <c r="F77" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G77" s="7"/>
-      <c r="H77" s="15"/>
+      <c r="H77" s="7"/>
       <c r="I77" s="15"/>
-      <c r="J77" s="7"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J77" s="15"/>
+      <c r="K77" s="7"/>
+      <c r="L77" s="15"/>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
       <c r="O77" s="15"/>
@@ -12227,7 +12303,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="78" spans="1:23" ht="50" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:23" ht="120" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>77</v>
       </c>
@@ -12240,15 +12316,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Joel 4:9–10</v>
       </c>
-      <c r="F78" s="7"/>
+      <c r="F78" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G78" s="7"/>
-      <c r="H78" s="15"/>
+      <c r="H78" s="7"/>
       <c r="I78" s="15"/>
-      <c r="J78" s="7"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J78" s="15"/>
+      <c r="K78" s="7"/>
+      <c r="L78" s="15"/>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
       <c r="O78" s="15"/>
@@ -12284,14 +12360,14 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Amos 3:4–5</v>
       </c>
-      <c r="F79" s="7"/>
+      <c r="F79" s="19"/>
       <c r="G79" s="7"/>
-      <c r="H79" s="15" t="s">
+      <c r="H79" s="7"/>
+      <c r="I79" s="15" t="s">
         <v>421</v>
       </c>
-      <c r="I79" s="15"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="19"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="8"/>
       <c r="L79" s="19"/>
       <c r="M79" s="19" t="s">
         <v>422</v>
@@ -12332,14 +12408,14 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.181 Amos1</v>
       </c>
-      <c r="F80" s="7"/>
-      <c r="G80" s="8" t="s">
+      <c r="F80" s="19"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="8" t="s">
         <v>426</v>
       </c>
-      <c r="H80" s="15"/>
       <c r="I80" s="15"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="19"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="8"/>
       <c r="L80" s="19"/>
       <c r="M80" s="15" t="s">
         <v>427</v>
@@ -12367,7 +12443,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="81" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>80</v>
       </c>
@@ -12380,15 +12456,15 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Obadiah 2:15, 16–18</v>
       </c>
-      <c r="F81" s="7"/>
-      <c r="G81" s="8"/>
-      <c r="H81" s="15"/>
+      <c r="F81" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G81" s="7"/>
+      <c r="H81" s="8"/>
       <c r="I81" s="15"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="19"/>
-      <c r="L81" s="19" t="s">
-        <v>45</v>
-      </c>
+      <c r="J81" s="15"/>
+      <c r="K81" s="8"/>
+      <c r="L81" s="19"/>
       <c r="M81" s="15"/>
       <c r="N81" s="15"/>
       <c r="O81" s="15"/>
@@ -12407,7 +12483,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="82" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>81</v>
       </c>
@@ -12424,14 +12500,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.197 Jon1</v>
       </c>
-      <c r="F82" s="7" t="s">
+      <c r="F82" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G82" s="7" t="s">
         <v>434</v>
       </c>
-      <c r="G82" s="7"/>
-      <c r="H82" s="15"/>
+      <c r="H82" s="7"/>
       <c r="I82" s="15"/>
-      <c r="J82" s="7"/>
-      <c r="K82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="7"/>
       <c r="L82" s="15"/>
       <c r="M82" s="15" t="s">
         <v>585</v>
@@ -12457,7 +12535,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="83" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:23" ht="80" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>82</v>
       </c>
@@ -12474,14 +12552,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.198 Mic1</v>
       </c>
-      <c r="F83" s="7" t="s">
+      <c r="F83" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G83" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="G83" s="7"/>
-      <c r="H83" s="15"/>
+      <c r="H83" s="7"/>
       <c r="I83" s="15"/>
-      <c r="J83" s="7"/>
-      <c r="K83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="7"/>
       <c r="L83" s="15"/>
       <c r="M83" s="15" t="s">
         <v>585</v>
@@ -12520,17 +12600,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Tob 7:1–3</v>
       </c>
-      <c r="F84" s="7"/>
-      <c r="G84" s="7" t="s">
+      <c r="F84" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G84" s="7"/>
+      <c r="H84" s="7" t="s">
         <v>443</v>
       </c>
-      <c r="H84" s="15"/>
       <c r="I84" s="15"/>
-      <c r="J84" s="7"/>
-      <c r="K84" s="15"/>
-      <c r="L84" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J84" s="15"/>
+      <c r="K84" s="7"/>
+      <c r="L84" s="15"/>
       <c r="M84" s="15"/>
       <c r="N84" s="15"/>
       <c r="O84" s="15"/>
@@ -12566,18 +12646,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.123 Tob1</v>
       </c>
-      <c r="F85" s="7" t="s">
+      <c r="F85" s="19" t="s">
+        <v>621</v>
+      </c>
+      <c r="G85" s="7" t="s">
         <v>446</v>
       </c>
-      <c r="G85" s="7"/>
-      <c r="H85" s="15"/>
-      <c r="I85" s="15" t="s">
+      <c r="H85" s="7"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15" t="s">
         <v>557</v>
       </c>
-      <c r="J85" s="9" t="s">
+      <c r="K85" s="9" t="s">
         <v>447</v>
       </c>
-      <c r="K85" s="19"/>
       <c r="L85" s="19"/>
       <c r="M85" s="15" t="s">
         <v>192</v>
@@ -12605,7 +12687,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="86" spans="1:23" ht="80" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:23" ht="190" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>85</v>
       </c>
@@ -12622,18 +12704,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.124 En1</v>
       </c>
-      <c r="F86" s="7" t="s">
+      <c r="F86" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G86" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="G86" s="7"/>
-      <c r="H86" s="15"/>
-      <c r="I86" s="15" t="s">
+      <c r="H86" s="7"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15" t="s">
         <v>558</v>
       </c>
-      <c r="J86" s="7" t="s">
+      <c r="K86" s="7" t="s">
         <v>453</v>
       </c>
-      <c r="K86" s="15"/>
       <c r="L86" s="15"/>
       <c r="M86" s="15" t="s">
         <v>52</v>
@@ -12676,23 +12760,25 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.125 En2</v>
       </c>
-      <c r="F87" s="7" t="s">
+      <c r="F87" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G87" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="G87" s="15" t="s">
+      <c r="H87" s="15" t="s">
         <v>459</v>
       </c>
-      <c r="H87" s="16" t="s">
+      <c r="I87" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="I87" s="15"/>
-      <c r="J87" s="9" t="s">
+      <c r="J87" s="15"/>
+      <c r="K87" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="K87" s="15" t="s">
+      <c r="L87" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="L87" s="15"/>
       <c r="M87" s="15" t="s">
         <v>597</v>
       </c>
@@ -12717,7 +12803,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="88" spans="1:23" ht="30" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:23" ht="60" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>87</v>
       </c>
@@ -12734,16 +12820,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.126 En3</v>
       </c>
-      <c r="F88" s="7" t="s">
+      <c r="F88" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G88" s="7" t="s">
         <v>466</v>
       </c>
-      <c r="G88" s="7"/>
-      <c r="H88" s="15"/>
+      <c r="H88" s="7"/>
       <c r="I88" s="15"/>
-      <c r="J88" s="9" t="s">
+      <c r="J88" s="15"/>
+      <c r="K88" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="K88" s="15"/>
       <c r="L88" s="15"/>
       <c r="M88" s="15" t="s">
         <v>468</v>
@@ -12771,7 +12859,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="89" spans="1:23" ht="200" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:23" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>88</v>
       </c>
@@ -12788,18 +12876,20 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.202 Instr1</v>
       </c>
-      <c r="F89" s="7" t="s">
+      <c r="F89" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G89" s="7" t="s">
         <v>472</v>
       </c>
-      <c r="G89" s="7"/>
-      <c r="H89" s="15"/>
-      <c r="I89" s="15" t="s">
+      <c r="H89" s="7"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15" t="s">
         <v>559</v>
       </c>
-      <c r="J89" s="7" t="s">
+      <c r="K89" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="K89" s="15"/>
       <c r="L89" s="15"/>
       <c r="M89" s="15" t="s">
         <v>586</v>
@@ -12844,17 +12934,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Instruction (“4Q418”)</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F90" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G90" s="7" t="s">
         <v>478</v>
       </c>
-      <c r="G90" s="7"/>
-      <c r="H90" s="15"/>
+      <c r="H90" s="7"/>
       <c r="I90" s="15"/>
-      <c r="J90" s="7"/>
-      <c r="K90" s="15"/>
-      <c r="L90" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="J90" s="15"/>
+      <c r="K90" s="7"/>
+      <c r="L90" s="15"/>
       <c r="M90" s="15"/>
       <c r="N90" s="15"/>
       <c r="O90" s="15"/>
@@ -12886,17 +12976,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Fragment with text from the Temple Scroll</v>
       </c>
-      <c r="F91" s="7"/>
+      <c r="F91" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G91" s="7"/>
-      <c r="H91" s="15"/>
-      <c r="I91" s="15" t="s">
+      <c r="H91" s="7"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15" t="s">
         <v>481</v>
       </c>
-      <c r="J91" s="7"/>
-      <c r="K91" s="15"/>
-      <c r="L91" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="K91" s="7"/>
+      <c r="L91" s="15"/>
       <c r="M91" s="15"/>
       <c r="N91" s="15"/>
       <c r="O91" s="15"/>
@@ -12926,17 +13016,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Fragment with text from the Temple Scroll</v>
       </c>
-      <c r="F92" s="7"/>
+      <c r="F92" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="G92" s="7"/>
-      <c r="H92" s="15"/>
-      <c r="I92" s="15" t="s">
+      <c r="H92" s="7"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15" t="s">
         <v>482</v>
       </c>
-      <c r="J92" s="7"/>
-      <c r="K92" s="15"/>
-      <c r="L92" s="15" t="s">
-        <v>45</v>
-      </c>
+      <c r="K92" s="7"/>
+      <c r="L92" s="15"/>
       <c r="M92" s="15"/>
       <c r="N92" s="15"/>
       <c r="O92" s="15"/>
@@ -12972,16 +13062,18 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.130 CommGen</v>
       </c>
-      <c r="F93" s="7" t="s">
+      <c r="F93" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G93" s="7" t="s">
         <v>486</v>
       </c>
-      <c r="G93" s="7"/>
-      <c r="H93" s="15"/>
-      <c r="I93" s="15" t="s">
+      <c r="H93" s="7"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="J93" s="7"/>
-      <c r="K93" s="15"/>
+      <c r="K93" s="7"/>
       <c r="L93" s="15"/>
       <c r="M93" s="15" t="s">
         <v>293</v>
@@ -13020,14 +13112,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v xml:space="preserve">DSS F.132 </v>
       </c>
-      <c r="F94" s="7" t="s">
+      <c r="F94" s="15" t="s">
+        <v>621</v>
+      </c>
+      <c r="G94" s="7" t="s">
         <v>490</v>
       </c>
-      <c r="G94" s="7"/>
-      <c r="H94" s="15"/>
+      <c r="H94" s="7"/>
       <c r="I94" s="15"/>
-      <c r="J94" s="7"/>
-      <c r="K94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="7"/>
       <c r="L94" s="15"/>
       <c r="M94" s="15" t="s">
         <v>598</v>
@@ -13068,16 +13162,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>DSS F.168 Text1</v>
       </c>
-      <c r="F95" s="7"/>
-      <c r="G95" s="7" t="s">
+      <c r="F95" s="15"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="7" t="s">
         <v>493</v>
       </c>
-      <c r="H95" s="15" t="s">
+      <c r="I95" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="I95" s="15"/>
-      <c r="J95" s="7"/>
-      <c r="K95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="7"/>
       <c r="L95" s="15"/>
       <c r="M95" s="15" t="s">
         <v>203</v>
@@ -13116,16 +13210,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F96" s="7" t="s">
+      <c r="F96" s="15"/>
+      <c r="G96" s="7" t="s">
         <v>496</v>
       </c>
-      <c r="G96" s="7" t="s">
+      <c r="H96" s="7" t="s">
         <v>544</v>
       </c>
-      <c r="H96" s="15"/>
       <c r="I96" s="15"/>
-      <c r="J96" s="7"/>
-      <c r="K96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="7"/>
       <c r="L96" s="15"/>
       <c r="M96" s="15" t="s">
         <v>497</v>
@@ -13162,17 +13256,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F97" s="7"/>
-      <c r="G97" s="7" t="s">
+      <c r="F97" s="15" t="s">
+        <v>599</v>
+      </c>
+      <c r="G97" s="7"/>
+      <c r="H97" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="H97" s="15"/>
       <c r="I97" s="15"/>
-      <c r="J97" s="7"/>
-      <c r="K97" s="15"/>
-      <c r="L97" s="15" t="s">
-        <v>599</v>
-      </c>
+      <c r="J97" s="15"/>
+      <c r="K97" s="7"/>
+      <c r="L97" s="15"/>
       <c r="M97" s="15"/>
       <c r="N97" s="15"/>
       <c r="O97" s="15"/>
@@ -13202,17 +13296,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F98" s="7"/>
-      <c r="G98" s="7" t="s">
+      <c r="F98" s="15" t="s">
+        <v>600</v>
+      </c>
+      <c r="G98" s="7"/>
+      <c r="H98" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="H98" s="15"/>
       <c r="I98" s="15"/>
-      <c r="J98" s="7"/>
-      <c r="K98" s="15"/>
-      <c r="L98" s="15" t="s">
-        <v>600</v>
-      </c>
+      <c r="J98" s="15"/>
+      <c r="K98" s="7"/>
+      <c r="L98" s="15"/>
       <c r="M98" s="15"/>
       <c r="N98" s="15"/>
       <c r="O98" s="15"/>
@@ -13229,7 +13323,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <v>98</v>
       </c>
@@ -13242,14 +13336,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F99" s="7" t="s">
+      <c r="F99" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G99" s="7" t="s">
         <v>501</v>
       </c>
-      <c r="G99" s="7"/>
-      <c r="H99" s="15"/>
+      <c r="H99" s="7"/>
       <c r="I99" s="15"/>
-      <c r="J99" s="7"/>
-      <c r="K99" s="15"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="7"/>
       <c r="L99" s="15"/>
       <c r="M99" s="15" t="s">
         <v>587</v>
@@ -13269,7 +13365,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>99</v>
       </c>
@@ -13282,14 +13378,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F100" s="7" t="s">
+      <c r="F100" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G100" s="7" t="s">
         <v>502</v>
       </c>
-      <c r="G100" s="7"/>
-      <c r="H100" s="15"/>
+      <c r="H100" s="7"/>
       <c r="I100" s="15"/>
-      <c r="J100" s="7"/>
-      <c r="K100" s="15"/>
+      <c r="J100" s="15"/>
+      <c r="K100" s="7"/>
       <c r="L100" s="15"/>
       <c r="M100" s="15" t="s">
         <v>588</v>
@@ -13309,7 +13407,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:23" ht="30" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <v>100</v>
       </c>
@@ -13322,14 +13420,16 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Unidentified</v>
       </c>
-      <c r="F101" s="7" t="s">
+      <c r="F101" s="15" t="s">
+        <v>620</v>
+      </c>
+      <c r="G101" s="7" t="s">
         <v>503</v>
       </c>
-      <c r="G101" s="7"/>
-      <c r="H101" s="15"/>
+      <c r="H101" s="7"/>
       <c r="I101" s="15"/>
-      <c r="J101" s="7"/>
-      <c r="K101" s="15"/>
+      <c r="J101" s="15"/>
+      <c r="K101" s="7"/>
       <c r="L101" s="15"/>
       <c r="M101" s="15" t="s">
         <v>588</v>
@@ -13349,7 +13449,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="45" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:23" ht="75" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>504</v>
       </c>
@@ -13362,17 +13462,17 @@
         <f>IF(ISNUMBER(Post_2002_Fragments[[#This Row],[No.]]),_xlfn.CONCAT(IF(Post_2002_Fragments[[#This Row],[DSS F. No.]]="",IF(ISNUMBER(SEARCH("Unidentified",Post_2002_Fragments[[#This Row],[Content]])),"Unidentified",Post_2002_Fragments[[#This Row],[Content]]),_xlfn.CONCAT("DSS F.",Post_2002_Fragments[[#This Row],[DSS F. No.]]," ",Post_2002_Fragments[[#This Row],[DSS F. Name]]))),Post_2002_Fragments[[#This Row],[No.]])</f>
         <v>Scraps</v>
       </c>
-      <c r="F102" s="7"/>
-      <c r="G102" s="7" t="s">
+      <c r="F102" s="15" t="s">
+        <v>601</v>
+      </c>
+      <c r="G102" s="7"/>
+      <c r="H102" s="7" t="s">
         <v>506</v>
       </c>
-      <c r="H102" s="15"/>
       <c r="I102" s="15"/>
-      <c r="J102" s="7"/>
-      <c r="K102" s="15"/>
-      <c r="L102" s="15" t="s">
-        <v>601</v>
-      </c>
+      <c r="J102" s="15"/>
+      <c r="K102" s="7"/>
+      <c r="L102" s="15"/>
       <c r="M102" s="15" t="s">
         <v>507</v>
       </c>
@@ -13396,9 +13496,9 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I59" r:id="rId1" location="v=onepage&amp;q=Sch%C3%B8yen&amp;f=false" display="https://books.google.no/books?id=Cs3RAgAAQBAJ&amp;pg=PA238&amp;lpg=PA238&amp;dq=PSALMS+DEAD+SEA+SCROLL+schoyen&amp;source=bl&amp;ots=9S5NHKbhNy&amp;sig=D1Mzi1d85boxzbk6tQCqiCZeEzw&amp;hl=no&amp;sa=X&amp;ei=7SVGVb-yO8KfsAGa_oHADw&amp;ved=0CFAQ6AEwBw - v=onepage&amp;q=Sch%C3%B8yen&amp;f=false" xr:uid="{151E52F6-AC3D-8948-A541-40365B388144}"/>
+    <hyperlink ref="J59" r:id="rId1" location="v=onepage&amp;q=Sch%C3%B8yen&amp;f=false" display="https://books.google.no/books?id=Cs3RAgAAQBAJ&amp;pg=PA238&amp;lpg=PA238&amp;dq=PSALMS+DEAD+SEA+SCROLL+schoyen&amp;source=bl&amp;ots=9S5NHKbhNy&amp;sig=D1Mzi1d85boxzbk6tQCqiCZeEzw&amp;hl=no&amp;sa=X&amp;ei=7SVGVb-yO8KfsAGa_oHADw&amp;ved=0CFAQ6AEwBw - v=onepage&amp;q=Sch%C3%B8yen&amp;f=false" xr:uid="{151E52F6-AC3D-8948-A541-40365B388144}"/>
     <hyperlink ref="M79" r:id="rId2" display="https://web.archive.org/web/20131011210336/http:/www.thekjvbible.com:80/onlinegallery/12/Dead+Sea+Scroll+Fragment" xr:uid="{A577A659-34A1-C34E-84ED-B965268DAB71}"/>
-    <hyperlink ref="G80" r:id="rId3" display="http://web.archive.org/web/20131229042349/http:/www.laniertheologicallibrary.org/original-dead-sea-scrolls-fragment-on-display/" xr:uid="{795B567B-2EAD-F743-B40F-F257B05A4EA7}"/>
+    <hyperlink ref="H80" r:id="rId3" display="http://web.archive.org/web/20131229042349/http:/www.laniertheologicallibrary.org/original-dead-sea-scrolls-fragment-on-display/" xr:uid="{795B567B-2EAD-F743-B40F-F257B05A4EA7}"/>
     <hyperlink ref="R40" r:id="rId4" display="http://shomron0.tripod.com/2008/julyaugust.html" xr:uid="{1A0A489E-7295-B84B-BE6A-04624A263796}"/>
     <hyperlink ref="R43" r:id="rId5" location="metadata_info_tab_contents" display="Émile Puech, &quot;Notes sur le manuscrit des Juges 4Q50a,&quot; RevQ 21.2 (2003): 315–19" xr:uid="{C08DF31B-0D56-4381-B0A3-C8253DD349AA}"/>
   </hyperlinks>

</xml_diff>